<commit_message>
adding monitoring and fix minor bugs
</commit_message>
<xml_diff>
--- a/public/template/Template DSBS.xlsx
+++ b/public/template/Template DSBS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irfansbom\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\siemas\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660CC34F-DAEA-447C-8885-5621A327DA69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4855E558-DAA6-4D4D-B82F-3E864C46F9AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A4248E35-6AB9-4A80-BD22-FFD7242506AB}"/>
   </bookViews>
@@ -71,10 +71,10 @@
     <t>1601010010001</t>
   </si>
   <si>
-    <t>ade.rismansyah</t>
-  </si>
-  <si>
     <t>susenas</t>
+  </si>
+  <si>
+    <t>pcl01@bpssumsel.com</t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -128,6 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +446,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +456,7 @@
     <col min="3" max="3" width="5.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
@@ -508,14 +509,14 @@
       <c r="F2" s="3">
         <v>1001</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="H2">
         <v>80</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
styling and FIX DSBS Import mengikuti daftar dari pusat
</commit_message>
<xml_diff>
--- a/public/template/Template DSBS.xlsx
+++ b/public/template/Template DSBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\siemas\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4855E558-DAA6-4D4D-B82F-3E864C46F9AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01E8A2C-DD6B-4417-9B20-1B48F29CB7FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A4248E35-6AB9-4A80-BD22-FFD7242506AB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>KD KAB</t>
   </si>
@@ -62,19 +62,16 @@
     <t>01</t>
   </si>
   <si>
-    <t>010</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
-    <t>1601010010001</t>
-  </si>
-  <si>
     <t>susenas</t>
   </si>
   <si>
-    <t>pcl01@bpssumsel.com</t>
+    <t>idris@bps.go.id</t>
+  </si>
+  <si>
+    <t>093</t>
   </si>
 </sst>
 </file>
@@ -128,7 +125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +443,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,8 +453,8 @@
     <col min="3" max="3" width="5.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -495,28 +492,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1601093001001</v>
       </c>
       <c r="F2" s="3">
         <v>1001</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3">
         <v>80</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>